<commit_message>
Update Regeln für Erstellung und Modifikation von Stored Procedures in DataFactory.xlsx
Regel ergänzt zum indirekten Aufruf öffentlicher Prozeduren über Webclient
</commit_message>
<xml_diff>
--- a/3c. DataFactory - Data Input and Database Configuration/Configuration for Database/Regeln für Erstellung und Modifikation von Stored Procedures in DataFactory.xlsx
+++ b/3c. DataFactory - Data Input and Database Configuration/Configuration for Database/Regeln für Erstellung und Modifikation von Stored Procedures in DataFactory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DataFactory-Knowledge-Center\3c. DataFactory - Data Input and Database Configuration\Configuration for Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2034F3C9-092E-4423-827C-C343EA9C9D39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CF3E2A-0940-449A-B8ED-676BD4378B33}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15420" xr2:uid="{852AC9EA-D57C-4287-923F-53FD82F86DD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{852AC9EA-D57C-4287-923F-53FD82F86DD4}"/>
   </bookViews>
   <sheets>
     <sheet name="POST" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Tabellen</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Regeln für individuelle DataFactory Prozeduren, welche Daten schreiben</t>
+  </si>
+  <si>
+    <t>-&gt; wenn es auch mit Webclient funktionieren muss, müssen die genutzten öffentlichen Prozeduren kopiert werden als custom version und aus diesen die Prüfung des Transactusername und die Prüfung der Schreibrechte entfernt werden</t>
   </si>
 </sst>
 </file>
@@ -864,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF0394D-A4BB-457A-8B44-3B7D145A6FC3}">
-  <dimension ref="B2:D52"/>
+  <dimension ref="B2:D53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,85 +1020,90 @@
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="3"/>
+      <c r="C34" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>